<commit_message>
Updated insertrecord with insertdrug code
</commit_message>
<xml_diff>
--- a/Clinic DB info.xlsx
+++ b/Clinic DB info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a4c9eff54134c15/Documents/GitHub/Clinic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_989C8D7592B8952EE8F30DB4C44480E579AC5E62" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{86996D7E-F3EA-4C6E-A2F2-6377924F08E1}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="11_989C8D7592B8952EE8F30DB4C44480E579AC5E62" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E71F62C9-B385-446B-9805-896BB39D1806}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,20 +615,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -664,6 +650,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,8 +939,8 @@
   </sheetPr>
   <dimension ref="A1:D1045"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1009,603 +1009,603 @@
     <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="28" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="30" t="s">
+      <c r="D44" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="28" t="s">
+      <c r="A46" s="11"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="28" t="s">
+      <c r="A47" s="11"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="30" t="s">
+      <c r="C48" s="34"/>
+      <c r="D48" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="28" t="s">
+      <c r="A50" s="11"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="30" t="s">
+      <c r="A51" s="11"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
+      <c r="A52" s="23"/>
       <c r="B52" s="5"/>
       <c r="C52" s="7"/>
-      <c r="D52" s="30" t="s">
+      <c r="D52" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="35" t="s">
         <v>99</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="25" t="s">
+      <c r="D53" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="28" t="s">
+      <c r="A54" s="11"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="13"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="25" t="s">
+      <c r="D55" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="13"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="25" t="s">
+      <c r="D56" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
-      <c r="B57" s="14"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="37"/>
       <c r="C57" s="6"/>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="25" t="s">
+      <c r="D58" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
+      <c r="A59" s="23"/>
       <c r="B59" s="5"/>
       <c r="C59" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D59" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="25" t="s">
+      <c r="D60" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="B61" s="26"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="20"/>
       <c r="C61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="B62" s="26"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="20"/>
       <c r="C62" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="D62" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="17"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="28" t="s">
+      <c r="A63" s="11"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="22" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A64" s="17"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="28" t="s">
+      <c r="A64" s="11"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="29"/>
+      <c r="A65" s="23"/>
       <c r="B65" s="5"/>
       <c r="C65" s="7"/>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="25" t="s">
+      <c r="D66" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="28" t="s">
+      <c r="A67" s="11"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="17"/>
-      <c r="B68" s="26"/>
+      <c r="A68" s="11"/>
+      <c r="B68" s="20"/>
       <c r="C68" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="25" t="s">
+      <c r="D68" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="28" t="s">
+      <c r="A69" s="11"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="28" t="s">
+      <c r="A70" s="11"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="17"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="28" t="s">
+      <c r="A71" s="11"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="22" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="26"/>
+      <c r="A72" s="11"/>
+      <c r="B72" s="20"/>
       <c r="C72" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="25" t="s">
+      <c r="D72" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="5"/>
       <c r="C73" s="6"/>
-      <c r="D73" s="30" t="s">
+      <c r="D73" s="24" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="24" t="s">
+      <c r="A74" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="25" t="s">
+      <c r="D74" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="33"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="36" t="s">
+      <c r="A75" s="27"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="37"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="32"/>
+      <c r="A76" s="31"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="26"/>
     </row>
     <row r="77" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="37"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="32"/>
+      <c r="A77" s="31"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="26"/>
     </row>
     <row r="78" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="37"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="32"/>
+      <c r="A78" s="31"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="26"/>
     </row>
     <row r="79" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="37"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="32"/>
+      <c r="A79" s="31"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="26"/>
     </row>
     <row r="80" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
     </row>
     <row r="81" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
+      <c r="A81" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="C81" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B82" s="18" t="s">
+      <c r="B82" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C82" s="17" t="s">
+      <c r="C82" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="D82" s="12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B83" s="18" t="s">
+      <c r="B83" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D83" s="18" t="s">
+      <c r="D83" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
+      <c r="A84" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B84" s="18" t="s">
+      <c r="B84" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="C84" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D84" s="20" t="s">
+      <c r="D84" s="14" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A85" s="17" t="s">
+      <c r="A85" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="D86" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A87" s="17" t="s">
+      <c r="A87" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="C87" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D87" s="18" t="s">
+      <c r="D87" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A88" s="17" t="s">
+      <c r="A88" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C88" s="17" t="s">
+      <c r="C88" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D88" s="18" t="s">
+      <c r="D88" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B89" s="18" t="s">
+      <c r="B89" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C89" s="19" t="s">
+      <c r="C89" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D89" s="20" t="s">
+      <c r="D89" s="14" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B90" s="18" t="s">
+      <c r="B90" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A91" s="17" t="s">
+      <c r="A91" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B91" s="18" t="s">
+      <c r="B91" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A92" s="17" t="s">
+      <c r="A92" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B92" s="18" t="s">
+      <c r="B92" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
+      <c r="A93" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
+      <c r="A94" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B94" s="18" t="s">
+      <c r="B94" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B95" s="18" t="s">
+      <c r="B95" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
+      <c r="A96" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+      <c r="A97" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B97" s="18" t="s">
+      <c r="B97" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+      <c r="A98" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B98" s="18" t="s">
+      <c r="B98" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A99" s="17" t="s">
+      <c r="A99" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
+      <c r="A100" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B100" s="18" t="s">
+      <c r="B100" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
+      <c r="A101" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B101" s="18" t="s">
+      <c r="B101" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A102" s="17" t="s">
+      <c r="A102" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B102" s="18" t="s">
+      <c r="B102" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A103" s="17" t="s">
+      <c r="A103" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B103" s="18" t="s">
+      <c r="B103" s="12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A104" s="17" t="s">
+      <c r="A104" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B104" s="18" t="s">
+      <c r="B104" s="12" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>